<commit_message>
adicionado nova lib addexcelmult
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Nome</t>
   </si>
@@ -31,10 +31,7 @@
     <t>Endereco</t>
   </si>
   <si>
-    <t>Christyan</t>
-  </si>
-  <si>
-    <t>Joao</t>
+    <t>Pedro</t>
   </si>
   <si>
     <t>1</t>
@@ -46,7 +43,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>7</t>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -404,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -431,34 +428,17 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionado função ler planilha otimizando o programa
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -1,81 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="CadastroUsuario" sheetId="1" r:id="rId1"/>
+    <sheet name="CadastroUsuario" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="CadastroProduto" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Telefone</t>
-  </si>
-  <si>
-    <t>Cpf</t>
-  </si>
-  <si>
-    <t>Endereco</t>
-  </si>
-  <si>
-    <t>Pedro</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -98,26 +68,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -159,7 +205,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -191,9 +237,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -225,6 +289,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -400,48 +482,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Telefone</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cpf</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Endereco</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Pedro</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>categoria</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>produto</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>cor</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>precocompra</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>precovenda</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>estoque</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Sofá</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Estante</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionado o cadastro de vendas
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="CadastroUsuario" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="CadastroProduto" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Vendas" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="CadastroProduto" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -34,6 +35,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -45,12 +51,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -78,12 +99,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -489,7 +513,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -555,6 +579,103 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>categoria</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>produto</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>cor</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>qtd_venda</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Estante</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Estante</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Estante</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Estante</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Estante</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Estante</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -569,32 +690,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>categoria</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>produto</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>cor</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>precocompra</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>precovenda</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>estoque</t>
         </is>
@@ -630,26 +751,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+          <t>Estante</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>9</v>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionar a função verificaplanhila
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -1,57 +1,136 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\OneDrive\Documentos\João Pedro\Python\aplicativovendas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D056E9AA-CE58-4730-9CF1-32E1BC9CCB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CadastroUsuario" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="CadastroProduto" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="CadastroVenda" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="CadastroUsuario" sheetId="1" r:id="rId1"/>
+    <sheet name="CadastroProduto" sheetId="2" r:id="rId2"/>
+    <sheet name="CadastroVenda" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>Cpf</t>
+  </si>
+  <si>
+    <t>Endereco</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>produto</t>
+  </si>
+  <si>
+    <t>cor</t>
+  </si>
+  <si>
+    <t>precocompra</t>
+  </si>
+  <si>
+    <t>precovenda</t>
+  </si>
+  <si>
+    <t>estoque</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Sofá</t>
+  </si>
+  <si>
+    <t>Estante</t>
+  </si>
+  <si>
+    <t>sofa</t>
+  </si>
+  <si>
+    <t>barcelona</t>
+  </si>
+  <si>
+    <t>branco</t>
+  </si>
+  <si>
+    <t>barca</t>
+  </si>
+  <si>
+    <t>cinza</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -89,102 +168,34 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
   </tableStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -508,71 +519,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Nome</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Telefone</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Cpf</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Endereco</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Pedro</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -581,133 +566,214 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>categoria</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>produto</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>cor</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>precocompra</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>precovenda</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>estoque</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Sofá</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>5</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>4</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>9</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>5</v>
       </c>
-      <c r="G2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Estante</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>9</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>5</v>
       </c>
-      <c r="G3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Estante</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Estante</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
         <v>5</v>
       </c>
-      <c r="G4" t="n">
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
         <v>2902</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>8066</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>300</v>
+      </c>
+      <c r="E6">
+        <v>400</v>
+      </c>
+      <c r="F6">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>4362</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>200</v>
+      </c>
+      <c r="E7">
+        <v>600</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>4362</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>300</v>
+      </c>
+      <c r="E8">
+        <v>400</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>500</v>
+      </c>
+      <c r="E9">
+        <v>800</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>1204</v>
       </c>
     </row>
   </sheetData>
@@ -716,19 +782,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
incluido funcões de verificar existência do usuario
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\OneDrive\Documentos\João Pedro\Python\aplicativovendas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christyan\Desktop\Projeto Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D056E9AA-CE58-4730-9CF1-32E1BC9CCB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E442AC-E21A-4689-AF0E-3D89B54E3521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CadastroUsuario" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Nome</t>
   </si>
@@ -40,18 +40,6 @@
   </si>
   <si>
     <t>Pedro</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>9</t>
   </si>
   <si>
     <t>categoria</t>
@@ -111,10 +99,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -522,24 +507,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -547,21 +534,21 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -569,38 +556,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -620,7 +607,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -640,10 +627,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -663,13 +650,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -686,13 +673,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
       </c>
       <c r="D6">
         <v>300</v>
@@ -709,13 +696,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
       </c>
       <c r="D7">
         <v>200</v>
@@ -732,13 +719,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D8">
         <v>300</v>
@@ -755,13 +742,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <v>500</v>

</xml_diff>